<commit_message>
Subiendo ultimos cambios del servicio deleteCrew
</commit_message>
<xml_diff>
--- a/Tareas.xlsx
+++ b/Tareas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ailyn\Proyectos\EasyPOC\EasyPOC\REPOSITORIO POC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ailyn\TAREAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E75A4E4-1A58-4983-8CF5-A2D0EEE91014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3500199A-D2FD-4D4A-B1F2-EEB42441C42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6384" yWindow="600" windowWidth="17280" windowHeight="11028" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20052" yWindow="-408" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Noviembre" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="389">
   <si>
     <t>Coordinación con Fabricio para continuar documento de Buenas prácticas para la solicitud de CAU</t>
   </si>
@@ -1142,6 +1142,69 @@
   </si>
   <si>
     <t>Pruebas al servicio deleteCrew. No terminado</t>
+  </si>
+  <si>
+    <t>Probando integración de selenium con azure devOps</t>
+  </si>
+  <si>
+    <t>9:00-1239</t>
+  </si>
+  <si>
+    <t>12:39-1:39</t>
+  </si>
+  <si>
+    <t>1:39-6:00</t>
+  </si>
+  <si>
+    <t>Integración de selenium con azure devOps</t>
+  </si>
+  <si>
+    <t>9:00-10:37</t>
+  </si>
+  <si>
+    <t>Documentando integración de selenium con azure devOps</t>
+  </si>
+  <si>
+    <t>Pruebas al servicio DeleteCrew y subir NC a azure</t>
+  </si>
+  <si>
+    <t>10:37-12:00</t>
+  </si>
+  <si>
+    <t>12:00-12:15</t>
+  </si>
+  <si>
+    <t>Actualizar prioridad y severidad en azure. Subir version de Easy POC</t>
+  </si>
+  <si>
+    <t>Completar pruebas al servicio /api/Crew/GetFligthCrew</t>
+  </si>
+  <si>
+    <t>12:15-12:30</t>
+  </si>
+  <si>
+    <t>1:30-2:45</t>
+  </si>
+  <si>
+    <t>2:45-4:00</t>
+  </si>
+  <si>
+    <t>Pruebas en pasarela 5 con los muchachos de VB</t>
+  </si>
+  <si>
+    <t>Preparar documento con NC y subirlo al OneDrive</t>
+  </si>
+  <si>
+    <t>4:00-4:35</t>
+  </si>
+  <si>
+    <t>4:35-5:10</t>
+  </si>
+  <si>
+    <t>5:10-5:50</t>
+  </si>
+  <si>
+    <t>Subir NC a Azure devOps de eGate 5</t>
   </si>
 </sst>
 </file>
@@ -1648,7 +1711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1920,7 +1983,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2338,14 +2410,14 @@
       <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2356,7 +2428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>44872</v>
       </c>
@@ -2365,21 +2437,21 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>44873</v>
       </c>
@@ -2388,14 +2460,14 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>44874</v>
       </c>
@@ -2404,14 +2476,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>44875</v>
       </c>
@@ -2420,14 +2492,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24">
         <v>44876</v>
       </c>
@@ -2436,7 +2508,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>44879</v>
       </c>
@@ -2445,14 +2517,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="23"/>
       <c r="C13" s="23" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>44880</v>
       </c>
@@ -2461,14 +2533,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>44881</v>
       </c>
@@ -2479,7 +2551,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
         <v>30</v>
@@ -2488,7 +2560,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
         <v>32</v>
@@ -2497,7 +2569,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
         <v>33</v>
@@ -2506,7 +2578,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
         <v>34</v>
@@ -2515,7 +2587,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
         <v>35</v>
@@ -2524,7 +2596,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="19" t="s">
         <v>37</v>
@@ -2533,7 +2605,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>44882</v>
       </c>
@@ -2544,7 +2616,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
         <v>40</v>
@@ -2553,7 +2625,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="5" t="s">
         <v>41</v>
@@ -2562,7 +2634,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="5" t="s">
         <v>43</v>
@@ -2571,7 +2643,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="5" t="s">
         <v>44</v>
@@ -2580,7 +2652,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="5" t="s">
         <v>46</v>
@@ -2589,7 +2661,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="5" t="s">
         <v>48</v>
@@ -2598,7 +2670,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="5" t="s">
         <v>50</v>
@@ -2607,7 +2679,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="19" t="s">
         <v>52</v>
@@ -2616,7 +2688,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>44883</v>
       </c>
@@ -2627,7 +2699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="6" t="s">
         <v>10</v>
@@ -2636,7 +2708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="7" t="s">
         <v>9</v>
@@ -2645,7 +2717,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="8" t="s">
         <v>7</v>
@@ -2654,7 +2726,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="8" t="s">
         <v>11</v>
@@ -2663,7 +2735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="8" t="s">
         <v>13</v>
@@ -2672,7 +2744,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="6" t="s">
         <v>16</v>
@@ -2681,7 +2753,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="8" t="s">
         <v>17</v>
@@ -2690,7 +2762,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="8" t="s">
         <v>19</v>
@@ -2699,7 +2771,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="8" t="s">
         <v>21</v>
@@ -2708,7 +2780,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="8" t="s">
         <v>25</v>
@@ -2717,7 +2789,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="10" t="s">
         <v>23</v>
@@ -2726,7 +2798,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18"/>
       <c r="B44" s="23" t="s">
         <v>27</v>
@@ -2735,7 +2807,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>44886</v>
       </c>
@@ -2746,7 +2818,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" s="10" t="s">
         <v>70</v>
@@ -2755,7 +2827,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="B47" s="14" t="s">
         <v>71</v>
@@ -2764,7 +2836,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
       <c r="B48" s="14" t="s">
         <v>73</v>
@@ -2773,7 +2845,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
       <c r="B49" s="10" t="s">
         <v>74</v>
@@ -2782,7 +2854,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="30"/>
       <c r="B50" s="31" t="s">
         <v>77</v>
@@ -2791,7 +2863,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="20">
         <v>44887</v>
       </c>
@@ -2802,7 +2874,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="8" t="s">
         <v>80</v>
@@ -2811,7 +2883,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="B53" s="14" t="s">
         <v>83</v>
@@ -2820,7 +2892,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="B54" s="14" t="s">
         <v>85</v>
@@ -2829,7 +2901,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="27"/>
       <c r="B55" s="29" t="s">
         <v>84</v>
@@ -2838,7 +2910,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="18"/>
       <c r="B56" s="23" t="s">
         <v>96</v>
@@ -2847,7 +2919,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="35">
         <v>44888</v>
       </c>
@@ -2858,7 +2930,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
       <c r="B58" s="10" t="s">
         <v>90</v>
@@ -2867,7 +2939,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="9"/>
       <c r="B59" s="10" t="s">
         <v>92</v>
@@ -2876,7 +2948,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
       <c r="B60" s="14" t="s">
         <v>94</v>
@@ -2885,7 +2957,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="9"/>
       <c r="B61" s="14" t="s">
         <v>98</v>
@@ -2895,7 +2967,7 @@
       </c>
       <c r="G61" s="33"/>
     </row>
-    <row r="62" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
       <c r="B62" s="34" t="s">
         <v>100</v>
@@ -2904,7 +2976,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="20">
         <v>44889</v>
       </c>
@@ -2915,7 +2987,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="8" t="s">
         <v>103</v>
@@ -2924,7 +2996,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="18"/>
       <c r="B65" s="34" t="s">
         <v>104</v>
@@ -2933,7 +3005,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
         <v>44890</v>
       </c>
@@ -2944,7 +3016,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="9"/>
       <c r="B67" s="10" t="s">
         <v>40</v>
@@ -2953,7 +3025,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="18"/>
       <c r="B68" s="23" t="s">
         <v>106</v>
@@ -2962,7 +3034,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="40">
         <v>44893</v>
       </c>
@@ -2973,7 +3045,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="9"/>
       <c r="B70" s="10" t="s">
         <v>109</v>
@@ -2982,7 +3054,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="9"/>
       <c r="B71" s="10" t="s">
         <v>111</v>
@@ -2991,7 +3063,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="9"/>
       <c r="B72" s="10" t="s">
         <v>114</v>
@@ -3000,7 +3072,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="27"/>
       <c r="B73" s="28" t="s">
         <v>115</v>
@@ -3009,7 +3081,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="9"/>
       <c r="B74" s="10" t="s">
         <v>117</v>
@@ -3018,7 +3090,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="43"/>
       <c r="B75" s="44" t="s">
         <v>118</v>
@@ -3027,7 +3099,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="20">
         <v>44894</v>
       </c>
@@ -3038,7 +3110,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="8" t="s">
         <v>122</v>
@@ -3047,7 +3119,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="18"/>
       <c r="B78" s="23" t="s">
         <v>123</v>
@@ -3056,7 +3128,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="11">
         <v>44895</v>
       </c>
@@ -3067,7 +3139,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="8" t="s">
         <v>126</v>
@@ -3076,7 +3148,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="6" t="s">
         <v>127</v>
@@ -3085,7 +3157,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="9"/>
       <c r="B82" s="14" t="s">
         <v>128</v>
@@ -3111,14 +3183,14 @@
       <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="67.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="67.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
         <v>2</v>
       </c>
@@ -3129,7 +3201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>44896</v>
       </c>
@@ -3140,7 +3212,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
         <v>132</v>
@@ -3149,7 +3221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
         <v>133</v>
@@ -3158,7 +3230,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>44897</v>
       </c>
@@ -3169,7 +3241,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="8" t="s">
         <v>137</v>
@@ -3178,7 +3250,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="23" t="s">
         <v>139</v>
@@ -3187,7 +3259,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="49">
         <v>44900</v>
       </c>
@@ -3198,7 +3270,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="6" t="s">
         <v>143</v>
@@ -3207,7 +3279,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="6" t="s">
         <v>145</v>
@@ -3216,7 +3288,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="6" t="s">
         <v>147</v>
@@ -3225,7 +3297,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="8" t="s">
         <v>149</v>
@@ -3234,7 +3306,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="23" t="s">
         <v>150</v>
@@ -3243,7 +3315,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="49">
         <v>44901</v>
       </c>
@@ -3254,7 +3326,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="8" t="s">
         <v>154</v>
@@ -3263,7 +3335,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="6" t="s">
         <v>155</v>
@@ -3272,7 +3344,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="6" t="s">
         <v>157</v>
@@ -3281,7 +3353,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="8" t="s">
         <v>159</v>
@@ -3290,7 +3362,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="53"/>
       <c r="B19" s="54" t="s">
         <v>161</v>
@@ -3299,7 +3371,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="56"/>
       <c r="B20" s="57" t="s">
         <v>163</v>
@@ -3308,7 +3380,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="23" t="s">
         <v>165</v>
@@ -3317,7 +3389,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="49">
         <v>44172</v>
       </c>
@@ -3328,7 +3400,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="56"/>
       <c r="B23" s="58" t="s">
         <v>169</v>
@@ -3337,7 +3409,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="56"/>
       <c r="B24" s="57" t="s">
         <v>170</v>
@@ -3346,7 +3418,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="53"/>
       <c r="B25" s="54" t="s">
         <v>172</v>
@@ -3355,7 +3427,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="23" t="s">
         <v>174</v>
@@ -3364,7 +3436,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>44903</v>
       </c>
@@ -3375,7 +3447,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="6" t="s">
         <v>177</v>
@@ -3384,7 +3456,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="8" t="s">
         <v>179</v>
@@ -3393,7 +3465,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
       <c r="B30" s="23" t="s">
         <v>180</v>
@@ -3402,7 +3474,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
         <v>44904</v>
       </c>
@@ -3413,7 +3485,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="56"/>
       <c r="B32" s="61" t="s">
         <v>184</v>
@@ -3422,7 +3494,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="53"/>
       <c r="B33" s="54" t="s">
         <v>40</v>
@@ -3431,7 +3503,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="18"/>
       <c r="B34" s="34" t="s">
         <v>186</v>
@@ -3440,7 +3512,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="62">
         <v>44177</v>
       </c>
@@ -3451,7 +3523,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="8" t="s">
         <v>40</v>
@@ -3460,7 +3532,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="6" t="s">
         <v>190</v>
@@ -3469,7 +3541,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="6" t="s">
         <v>192</v>
@@ -3478,7 +3550,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="8" t="s">
         <v>194</v>
@@ -3487,7 +3559,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="56"/>
       <c r="B40" s="58" t="s">
         <v>196</v>
@@ -3496,7 +3568,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="20">
         <v>44908</v>
       </c>
@@ -3507,7 +3579,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="8" t="s">
         <v>200</v>
@@ -3516,7 +3588,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="56"/>
       <c r="B43" s="58" t="s">
         <v>202</v>
@@ -3525,7 +3597,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="8" t="s">
         <v>203</v>
@@ -3534,7 +3606,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="6" t="s">
         <v>204</v>
@@ -3543,7 +3615,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="8" t="s">
         <v>206</v>
@@ -3552,7 +3624,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18"/>
       <c r="B47" s="23" t="s">
         <v>208</v>
@@ -3561,7 +3633,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="20">
         <v>44909</v>
       </c>
@@ -3572,7 +3644,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="8" t="s">
         <v>184</v>
@@ -3581,7 +3653,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="8" t="s">
         <v>40</v>
@@ -3590,7 +3662,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18"/>
       <c r="B51" s="23" t="s">
         <v>186</v>
@@ -3599,7 +3671,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="64">
         <v>44910</v>
       </c>
@@ -3610,7 +3682,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="53"/>
       <c r="B53" s="54" t="s">
         <v>40</v>
@@ -3619,7 +3691,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="56"/>
       <c r="B54" s="58" t="s">
         <v>212</v>
@@ -3628,7 +3700,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="18"/>
       <c r="B55" s="23" t="s">
         <v>165</v>
@@ -3637,7 +3709,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="20">
         <v>44911</v>
       </c>
@@ -3648,7 +3720,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="8" t="s">
         <v>214</v>
@@ -3657,7 +3729,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="8" t="s">
         <v>216</v>
@@ -3666,7 +3738,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="8" t="s">
         <v>212</v>
@@ -3675,7 +3747,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="56"/>
       <c r="B60" s="58" t="s">
         <v>165</v>
@@ -3684,7 +3756,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="20">
         <v>44914</v>
       </c>
@@ -3695,7 +3767,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="56"/>
       <c r="B62" s="57" t="s">
         <v>218</v>
@@ -3704,7 +3776,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="53"/>
       <c r="B63" s="66" t="s">
         <v>220</v>
@@ -3713,7 +3785,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="8" t="s">
         <v>222</v>
@@ -3722,7 +3794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="18"/>
       <c r="B65" s="34" t="s">
         <v>223</v>
@@ -3731,7 +3803,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="69">
         <v>44915</v>
       </c>
@@ -3742,7 +3814,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="8" t="s">
         <v>40</v>
@@ -3751,7 +3823,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="56"/>
       <c r="B68" s="58" t="s">
         <v>212</v>
@@ -3760,7 +3832,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="18"/>
       <c r="B69" s="23" t="s">
         <v>165</v>
@@ -3769,7 +3841,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="20">
         <v>44916</v>
       </c>
@@ -3780,7 +3852,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="8" t="s">
         <v>228</v>
@@ -3789,7 +3861,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="8" t="s">
         <v>230</v>
@@ -3798,7 +3870,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="8" t="s">
         <v>232</v>
@@ -3807,7 +3879,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="8" t="s">
         <v>40</v>
@@ -3816,7 +3888,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="56"/>
       <c r="B75" s="57" t="s">
         <v>234</v>
@@ -3825,7 +3897,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="56"/>
       <c r="B76" s="58" t="s">
         <v>236</v>
@@ -3834,7 +3906,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="64">
         <v>44917</v>
       </c>
@@ -3845,7 +3917,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="8" t="s">
         <v>238</v>
@@ -3854,7 +3926,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="18"/>
       <c r="B79" s="23" t="s">
         <v>150</v>
@@ -3863,7 +3935,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="20">
         <v>44918</v>
       </c>
@@ -3874,7 +3946,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="68" t="s">
         <v>243</v>
@@ -3883,7 +3955,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="8" t="s">
         <v>244</v>
@@ -3892,7 +3964,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="8" t="s">
         <v>246</v>
@@ -3901,7 +3973,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="6" t="s">
         <v>248</v>
@@ -3910,7 +3982,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="56"/>
       <c r="B85" s="58" t="s">
         <v>249</v>
@@ -3919,7 +3991,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="20">
         <v>44921</v>
       </c>
@@ -3930,7 +4002,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="8" t="s">
         <v>40</v>
@@ -3939,7 +4011,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="56"/>
       <c r="B88" s="57" t="s">
         <v>251</v>
@@ -3948,7 +4020,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="20">
         <v>44922</v>
       </c>
@@ -3959,7 +4031,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="6" t="s">
         <v>253</v>
@@ -3968,7 +4040,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="8" t="s">
         <v>255</v>
@@ -3977,7 +4049,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="56"/>
       <c r="B92" s="57" t="s">
         <v>256</v>
@@ -3986,7 +4058,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="8" t="s">
         <v>258</v>
@@ -3995,7 +4067,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="18"/>
       <c r="B94" s="23" t="s">
         <v>260</v>
@@ -4004,7 +4076,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="20">
         <v>44923</v>
       </c>
@@ -4015,7 +4087,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="8" t="s">
         <v>184</v>
@@ -4024,7 +4096,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="8" t="s">
         <v>40</v>
@@ -4033,7 +4105,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="8" t="s">
         <v>266</v>
@@ -4042,7 +4114,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="6" t="s">
         <v>268</v>
@@ -4051,7 +4123,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="18"/>
       <c r="B100" s="23" t="s">
         <v>165</v>
@@ -4060,7 +4132,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="20">
         <v>44924</v>
       </c>
@@ -4071,7 +4143,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="8" t="s">
         <v>270</v>
@@ -4080,7 +4152,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="18"/>
       <c r="B103" s="23" t="s">
         <v>165</v>
@@ -4089,7 +4161,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="49">
         <v>44925</v>
       </c>
@@ -4100,7 +4172,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" s="8" t="s">
         <v>149</v>
@@ -4109,7 +4181,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="6" t="s">
         <v>273</v>
@@ -4125,20 +4197,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80819AD-073B-4223-840B-D30427A93CF6}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="40.109375" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="72" t="s">
         <v>2</v>
       </c>
@@ -4149,7 +4221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="74">
         <v>44928</v>
       </c>
@@ -4160,7 +4232,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="77"/>
       <c r="B3" s="5" t="s">
         <v>277</v>
@@ -4169,7 +4241,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="77"/>
       <c r="B4" s="48" t="s">
         <v>279</v>
@@ -4178,7 +4250,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="79"/>
       <c r="B5" s="71" t="s">
         <v>281</v>
@@ -4187,7 +4259,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="79"/>
       <c r="B6" s="71" t="s">
         <v>282</v>
@@ -4196,7 +4268,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="79"/>
       <c r="B7" t="s">
         <v>285</v>
@@ -4205,7 +4277,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="79"/>
       <c r="B8" s="70" t="s">
         <v>283</v>
@@ -4214,7 +4286,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="79"/>
       <c r="B9" s="71" t="s">
         <v>289</v>
@@ -4224,7 +4296,7 @@
       </c>
       <c r="G9" s="33"/>
     </row>
-    <row r="10" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="83"/>
       <c r="B10" s="84" t="s">
         <v>290</v>
@@ -4233,7 +4305,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="87">
         <v>44929</v>
       </c>
@@ -4244,7 +4316,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="79"/>
       <c r="B12" s="70" t="s">
         <v>149</v>
@@ -4253,7 +4325,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="79"/>
       <c r="B13" s="86" t="s">
         <v>294</v>
@@ -4262,7 +4334,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="100"/>
       <c r="B14" s="97" t="s">
         <v>165</v>
@@ -4271,7 +4343,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="94">
         <v>44930</v>
       </c>
@@ -4282,7 +4354,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="90"/>
       <c r="B16" s="98" t="s">
         <v>298</v>
@@ -4291,7 +4363,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="90"/>
       <c r="B17" s="99" t="s">
         <v>301</v>
@@ -4300,7 +4372,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="90"/>
       <c r="B18" s="98" t="s">
         <v>132</v>
@@ -4309,7 +4381,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="90"/>
       <c r="B19" s="98" t="s">
         <v>303</v>
@@ -4318,7 +4390,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="90"/>
       <c r="B20" s="98" t="s">
         <v>304</v>
@@ -4327,7 +4399,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="90"/>
       <c r="B21" s="99" t="s">
         <v>307</v>
@@ -4336,7 +4408,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="94">
         <v>44931</v>
       </c>
@@ -4347,7 +4419,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="90"/>
       <c r="B23" s="98" t="s">
         <v>184</v>
@@ -4356,7 +4428,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="90"/>
       <c r="B24" s="98" t="s">
         <v>311</v>
@@ -4365,7 +4437,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="91"/>
       <c r="B25" s="103" t="s">
         <v>165</v>
@@ -4374,7 +4446,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="94">
         <v>44935</v>
       </c>
@@ -4385,7 +4457,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="90"/>
       <c r="B27" s="98" t="s">
         <v>315</v>
@@ -4394,7 +4466,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="90"/>
       <c r="B28" s="99" t="s">
         <v>317</v>
@@ -4403,7 +4475,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="90"/>
       <c r="B29" s="99" t="s">
         <v>318</v>
@@ -4412,7 +4484,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="90"/>
       <c r="B30" s="98" t="s">
         <v>149</v>
@@ -4421,7 +4493,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="90"/>
       <c r="B31" s="99" t="s">
         <v>320</v>
@@ -4430,7 +4502,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="91"/>
       <c r="B32" s="103" t="s">
         <v>321</v>
@@ -4439,7 +4511,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="94">
         <v>44936</v>
       </c>
@@ -4450,7 +4522,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="90"/>
       <c r="B34" s="98" t="s">
         <v>132</v>
@@ -4459,7 +4531,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="90"/>
       <c r="B35" s="99" t="s">
         <v>325</v>
@@ -4468,7 +4540,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="90"/>
       <c r="B36" s="99" t="s">
         <v>249</v>
@@ -4477,7 +4549,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="94">
         <v>44937</v>
       </c>
@@ -4488,7 +4560,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="90"/>
       <c r="B38" s="98" t="s">
         <v>329</v>
@@ -4497,7 +4569,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="90"/>
       <c r="B39" s="98" t="s">
         <v>330</v>
@@ -4506,7 +4578,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="90"/>
       <c r="B40" s="98" t="s">
         <v>331</v>
@@ -4515,7 +4587,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="90"/>
       <c r="B41" s="99" t="s">
         <v>332</v>
@@ -4524,7 +4596,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="90"/>
       <c r="B42" s="98" t="s">
         <v>333</v>
@@ -4533,7 +4605,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="90"/>
       <c r="B43" s="98" t="s">
         <v>165</v>
@@ -4542,7 +4614,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="94">
         <v>44938</v>
       </c>
@@ -4553,7 +4625,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="90"/>
       <c r="B45" s="98" t="s">
         <v>337</v>
@@ -4562,7 +4634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="90"/>
       <c r="B46" s="98" t="s">
         <v>338</v>
@@ -4571,7 +4643,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="90"/>
       <c r="B47" s="99" t="s">
         <v>341</v>
@@ -4580,7 +4652,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="90"/>
       <c r="B48" s="99" t="s">
         <v>343</v>
@@ -4589,7 +4661,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="91"/>
       <c r="B49" s="103" t="s">
         <v>344</v>
@@ -4598,7 +4670,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="94">
         <v>44939</v>
       </c>
@@ -4609,7 +4681,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="90"/>
       <c r="B51" s="98" t="s">
         <v>347</v>
@@ -4618,7 +4690,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="90"/>
       <c r="B52" s="98" t="s">
         <v>348</v>
@@ -4627,7 +4699,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="90"/>
       <c r="B53" s="98" t="s">
         <v>350</v>
@@ -4636,7 +4708,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="90"/>
       <c r="B54" s="98" t="s">
         <v>351</v>
@@ -4645,7 +4717,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="90"/>
       <c r="B55" s="98" t="s">
         <v>353</v>
@@ -4654,7 +4726,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="94">
         <v>44942</v>
       </c>
@@ -4665,7 +4737,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="90"/>
       <c r="B57" s="99" t="s">
         <v>358</v>
@@ -4674,7 +4746,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="90"/>
       <c r="B58" s="99" t="s">
         <v>362</v>
@@ -4683,7 +4755,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="90"/>
       <c r="B59" s="98" t="s">
         <v>360</v>
@@ -4692,7 +4764,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="90"/>
       <c r="B60" s="99" t="s">
         <v>363</v>
@@ -4701,7 +4773,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="90"/>
       <c r="B61" s="98" t="s">
         <v>364</v>
@@ -4710,7 +4782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="90"/>
       <c r="B62" s="99" t="s">
         <v>365</v>
@@ -4719,13 +4791,135 @@
         <v>366</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="91"/>
-      <c r="B63" s="107" t="s">
+    <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="90"/>
+      <c r="B63" s="99" t="s">
         <v>165</v>
       </c>
-      <c r="C63" s="102" t="s">
+      <c r="C63" s="93" t="s">
         <v>367</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="94">
+        <v>44943</v>
+      </c>
+      <c r="B64" s="104" t="s">
+        <v>369</v>
+      </c>
+      <c r="C64" s="95" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="90"/>
+      <c r="B65" s="98" t="s">
+        <v>370</v>
+      </c>
+      <c r="C65" s="93" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="90"/>
+      <c r="B66" s="99" t="s">
+        <v>371</v>
+      </c>
+      <c r="C66" s="96" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="94">
+        <v>44944</v>
+      </c>
+      <c r="B67" s="92" t="s">
+        <v>373</v>
+      </c>
+      <c r="C67" s="95" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="90"/>
+      <c r="B68" s="99" t="s">
+        <v>376</v>
+      </c>
+      <c r="C68" s="96" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="90"/>
+      <c r="B69" s="98" t="s">
+        <v>377</v>
+      </c>
+      <c r="C69" s="96" t="s">
+        <v>378</v>
+      </c>
+      <c r="D69" s="107"/>
+    </row>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="90"/>
+      <c r="B70" s="99" t="s">
+        <v>380</v>
+      </c>
+      <c r="C70" s="96" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="90"/>
+      <c r="B71" s="98" t="s">
+        <v>132</v>
+      </c>
+      <c r="C71" s="93" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="90"/>
+      <c r="B72" s="98" t="s">
+        <v>381</v>
+      </c>
+      <c r="C72" s="108" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="90"/>
+      <c r="B73" s="98" t="s">
+        <v>382</v>
+      </c>
+      <c r="C73" s="96" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="90"/>
+      <c r="B74" s="98" t="s">
+        <v>385</v>
+      </c>
+      <c r="C74" s="96" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="90"/>
+      <c r="B75" s="98" t="s">
+        <v>386</v>
+      </c>
+      <c r="C75" s="93" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="91"/>
+      <c r="B76" s="110" t="s">
+        <v>387</v>
+      </c>
+      <c r="C76" s="109" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>